<commit_message>
add new data files
</commit_message>
<xml_diff>
--- a/powerapp/data/dp_hvcb.xlsx
+++ b/powerapp/data/dp_hvcb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/externalDrive/code-gym/work/powerapp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myIjat\Dojo\power_app\powerapp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61086A6A-90EA-F240-9E06-0C63C0E7391A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7BD44E-23B4-4FE2-A124-3266B32F2FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9380" yWindow="920" windowWidth="19360" windowHeight="26380" xr2:uid="{85779A08-F2D4-4AB6-BDDB-4C6BF28C40BE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{85779A08-F2D4-4AB6-BDDB-4C6BF28C40BE}"/>
   </bookViews>
   <sheets>
     <sheet name="ls_hvcb_dp" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="302">
   <si>
     <t>feeder_id</t>
   </si>
@@ -915,6 +915,36 @@
   </si>
   <si>
     <t>ESTL</t>
+  </si>
+  <si>
+    <t>ssun_132</t>
+  </si>
+  <si>
+    <t>kbek_132</t>
+  </si>
+  <si>
+    <t>nsci_132</t>
+  </si>
+  <si>
+    <t>xnss_132</t>
+  </si>
+  <si>
+    <t>lkjg_132</t>
+  </si>
+  <si>
+    <t>ksni_132</t>
+  </si>
+  <si>
+    <t>utmj_132</t>
+  </si>
+  <si>
+    <t>kcmt_132</t>
+  </si>
+  <si>
+    <t>tpau_132</t>
+  </si>
+  <si>
+    <t>pltg_230</t>
   </si>
 </sst>
 </file>
@@ -924,7 +954,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1347,11 +1377,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D5A47D-D33D-415C-BB2B-6C65B298EFEB}">
   <dimension ref="A1:F276"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="A262" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="F271" sqref="F271"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="15.83203125" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" style="8" bestFit="1" customWidth="1"/>
@@ -1362,7 +1392,7 @@
     <col min="7" max="16384" width="8.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>116</v>
       </c>
@@ -1382,7 +1412,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>226</v>
       </c>
@@ -1402,7 +1432,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>226</v>
       </c>
@@ -1422,7 +1452,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" s="3" customFormat="1">
       <c r="A4" s="3" t="s">
         <v>228</v>
       </c>
@@ -1442,7 +1472,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>230</v>
       </c>
@@ -1462,7 +1492,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" s="3" customFormat="1">
       <c r="A6" s="3" t="s">
         <v>230</v>
       </c>
@@ -1482,7 +1512,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" s="3" customFormat="1">
       <c r="A7" s="3" t="s">
         <v>232</v>
       </c>
@@ -1502,7 +1532,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" s="3" customFormat="1">
       <c r="A8" s="3" t="s">
         <v>232</v>
       </c>
@@ -1522,7 +1552,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" s="3" customFormat="1">
       <c r="A9" s="3" t="s">
         <v>234</v>
       </c>
@@ -1542,7 +1572,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" s="3" customFormat="1">
       <c r="A10" s="3" t="s">
         <v>234</v>
       </c>
@@ -1562,7 +1592,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" s="3" customFormat="1">
       <c r="A11" s="3" t="s">
         <v>238</v>
       </c>
@@ -1582,7 +1612,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" s="3" customFormat="1">
       <c r="A12" s="3" t="s">
         <v>238</v>
       </c>
@@ -1602,7 +1632,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" s="3" customFormat="1">
       <c r="A13" s="3" t="s">
         <v>240</v>
       </c>
@@ -1622,7 +1652,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" s="3" customFormat="1">
       <c r="A14" s="3" t="s">
         <v>240</v>
       </c>
@@ -1642,7 +1672,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" s="3" customFormat="1">
       <c r="A15" s="3" t="s">
         <v>242</v>
       </c>
@@ -1662,7 +1692,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" s="3" customFormat="1">
       <c r="A16" s="3" t="s">
         <v>242</v>
       </c>
@@ -1682,7 +1712,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" s="3" customFormat="1">
       <c r="A17" s="3" t="s">
         <v>246</v>
       </c>
@@ -1702,7 +1732,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" s="3" customFormat="1">
       <c r="A18" s="3" t="s">
         <v>246</v>
       </c>
@@ -1722,7 +1752,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" s="3" customFormat="1">
       <c r="A19" s="3" t="s">
         <v>248</v>
       </c>
@@ -1742,7 +1772,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" s="3" customFormat="1">
       <c r="A20" s="3" t="s">
         <v>250</v>
       </c>
@@ -1762,7 +1792,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" s="3" customFormat="1">
       <c r="A21" s="3" t="s">
         <v>252</v>
       </c>
@@ -1782,7 +1812,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" s="3" customFormat="1">
       <c r="A22" s="3" t="s">
         <v>252</v>
       </c>
@@ -1802,7 +1832,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" s="3" customFormat="1">
       <c r="A23" s="3" t="s">
         <v>256</v>
       </c>
@@ -1822,7 +1852,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" s="3" customFormat="1">
       <c r="A24" s="3" t="s">
         <v>257</v>
       </c>
@@ -1842,7 +1872,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" s="3" customFormat="1">
       <c r="A25" s="3" t="s">
         <v>259</v>
       </c>
@@ -1862,7 +1892,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" s="3" customFormat="1">
       <c r="A26" s="3" t="s">
         <v>259</v>
       </c>
@@ -1882,7 +1912,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" s="3" customFormat="1">
       <c r="A27" s="3" t="s">
         <v>290</v>
       </c>
@@ -1900,7 +1930,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" s="3" customFormat="1">
       <c r="A28" s="3" t="s">
         <v>290</v>
       </c>
@@ -1918,7 +1948,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" s="5" t="s">
         <v>15</v>
       </c>
@@ -1938,7 +1968,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" s="5" t="s">
         <v>15</v>
       </c>
@@ -1958,7 +1988,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" s="3" t="s">
         <v>17</v>
       </c>
@@ -1978,7 +2008,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" s="3" t="s">
         <v>17</v>
       </c>
@@ -1998,7 +2028,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" s="3" t="s">
         <v>17</v>
       </c>
@@ -2018,7 +2048,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6">
       <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
@@ -2038,7 +2068,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" s="3" t="s">
         <v>17</v>
       </c>
@@ -2058,7 +2088,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" s="3" t="s">
         <v>17</v>
       </c>
@@ -2078,7 +2108,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" s="5" t="s">
         <v>21</v>
       </c>
@@ -2098,7 +2128,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" s="5" t="s">
         <v>21</v>
       </c>
@@ -2118,7 +2148,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" s="5" t="s">
         <v>21</v>
       </c>
@@ -2138,7 +2168,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40" s="5" t="s">
         <v>21</v>
       </c>
@@ -2158,7 +2188,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" s="5" t="s">
         <v>21</v>
       </c>
@@ -2178,7 +2208,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42" s="5" t="s">
         <v>21</v>
       </c>
@@ -2198,7 +2228,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" s="5" t="s">
         <v>21</v>
       </c>
@@ -2218,7 +2248,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6">
       <c r="A44" s="5" t="s">
         <v>21</v>
       </c>
@@ -2238,7 +2268,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45" s="5" t="s">
         <v>21</v>
       </c>
@@ -2258,7 +2288,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46" s="5" t="s">
         <v>27</v>
       </c>
@@ -2278,7 +2308,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6">
       <c r="A47" s="5" t="s">
         <v>27</v>
       </c>
@@ -2298,7 +2328,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6">
       <c r="A48" s="5" t="s">
         <v>27</v>
       </c>
@@ -2318,7 +2348,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6">
       <c r="A49" s="5" t="s">
         <v>27</v>
       </c>
@@ -2338,7 +2368,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6">
       <c r="A50" s="5" t="s">
         <v>27</v>
       </c>
@@ -2358,7 +2388,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6">
       <c r="A51" s="5" t="s">
         <v>27</v>
       </c>
@@ -2378,7 +2408,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6">
       <c r="A52" s="5" t="s">
         <v>27</v>
       </c>
@@ -2398,7 +2428,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6">
       <c r="A53" s="5" t="s">
         <v>27</v>
       </c>
@@ -2418,7 +2448,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6">
       <c r="A54" s="5" t="s">
         <v>27</v>
       </c>
@@ -2434,8 +2464,11 @@
       <c r="E54" s="10" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F54" s="7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" s="5" t="s">
         <v>27</v>
       </c>
@@ -2451,8 +2484,11 @@
       <c r="E55" s="10" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F55" s="7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" s="5" t="s">
         <v>30</v>
       </c>
@@ -2472,7 +2508,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6">
       <c r="A57" s="5" t="s">
         <v>30</v>
       </c>
@@ -2492,7 +2528,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6">
       <c r="A58" s="5" t="s">
         <v>30</v>
       </c>
@@ -2512,7 +2548,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6">
       <c r="A59" s="5" t="s">
         <v>30</v>
       </c>
@@ -2532,7 +2568,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6">
       <c r="A60" s="5" t="s">
         <v>30</v>
       </c>
@@ -2552,7 +2588,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6">
       <c r="A61" s="5" t="s">
         <v>30</v>
       </c>
@@ -2572,7 +2608,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6">
       <c r="A62" s="5" t="s">
         <v>30</v>
       </c>
@@ -2592,7 +2628,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6">
       <c r="A63" s="5" t="s">
         <v>30</v>
       </c>
@@ -2612,7 +2648,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6">
       <c r="A64" s="5" t="s">
         <v>30</v>
       </c>
@@ -2632,7 +2668,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6">
       <c r="A65" s="5" t="s">
         <v>30</v>
       </c>
@@ -2652,7 +2688,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6">
       <c r="A66" s="5" t="s">
         <v>30</v>
       </c>
@@ -2672,7 +2708,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6">
       <c r="A67" s="5" t="s">
         <v>30</v>
       </c>
@@ -2692,7 +2728,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6">
       <c r="A68" s="5" t="s">
         <v>30</v>
       </c>
@@ -2712,7 +2748,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6">
       <c r="A69" s="5" t="s">
         <v>30</v>
       </c>
@@ -2732,7 +2768,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6">
       <c r="A70" s="5" t="s">
         <v>30</v>
       </c>
@@ -2752,7 +2788,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6">
       <c r="A71" s="5" t="s">
         <v>30</v>
       </c>
@@ -2772,7 +2808,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6">
       <c r="A72" s="5" t="s">
         <v>30</v>
       </c>
@@ -2792,7 +2828,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6">
       <c r="A73" s="5" t="s">
         <v>39</v>
       </c>
@@ -2812,7 +2848,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6">
       <c r="A74" s="5" t="s">
         <v>39</v>
       </c>
@@ -2832,7 +2868,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6">
       <c r="A75" s="5" t="s">
         <v>39</v>
       </c>
@@ -2846,8 +2882,11 @@
         <v>8</v>
       </c>
       <c r="E75" s="10"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F75" s="7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76" s="5" t="s">
         <v>39</v>
       </c>
@@ -2861,8 +2900,11 @@
         <v>10</v>
       </c>
       <c r="E76" s="10"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F76" s="7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
       <c r="A77" s="5" t="s">
         <v>39</v>
       </c>
@@ -2882,7 +2924,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6">
       <c r="A78" s="5" t="s">
         <v>39</v>
       </c>
@@ -2902,7 +2944,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6">
       <c r="A79" s="5" t="s">
         <v>39</v>
       </c>
@@ -2922,7 +2964,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6">
       <c r="A80" s="5" t="s">
         <v>39</v>
       </c>
@@ -2942,7 +2984,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6">
       <c r="A81" s="5" t="s">
         <v>39</v>
       </c>
@@ -2962,7 +3004,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6">
       <c r="A82" s="5" t="s">
         <v>39</v>
       </c>
@@ -2982,7 +3024,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6">
       <c r="A83" s="5" t="s">
         <v>39</v>
       </c>
@@ -3002,7 +3044,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" ht="14.5" customHeight="1">
       <c r="A84" s="5" t="s">
         <v>39</v>
       </c>
@@ -3022,7 +3064,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" ht="14.5" customHeight="1">
       <c r="A85" s="5" t="s">
         <v>39</v>
       </c>
@@ -3042,7 +3084,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" ht="14.5" customHeight="1">
       <c r="A86" s="5" t="s">
         <v>39</v>
       </c>
@@ -3062,7 +3104,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" ht="14.5" customHeight="1">
       <c r="A87" s="5" t="s">
         <v>39</v>
       </c>
@@ -3082,7 +3124,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" ht="14.5" customHeight="1">
       <c r="A88" s="5" t="s">
         <v>39</v>
       </c>
@@ -3102,7 +3144,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" ht="14.5" customHeight="1">
       <c r="A89" s="5" t="s">
         <v>39</v>
       </c>
@@ -3122,7 +3164,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" ht="14.5" customHeight="1">
       <c r="A90" s="5" t="s">
         <v>39</v>
       </c>
@@ -3142,7 +3184,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" ht="14.5" customHeight="1">
       <c r="A91" s="5" t="s">
         <v>39</v>
       </c>
@@ -3162,7 +3204,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" ht="14.5" customHeight="1">
       <c r="A92" s="5" t="s">
         <v>39</v>
       </c>
@@ -3182,7 +3224,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" ht="14.5" customHeight="1">
       <c r="A93" s="5" t="s">
         <v>39</v>
       </c>
@@ -3202,7 +3244,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" ht="14.5" customHeight="1">
       <c r="A94" s="5" t="s">
         <v>39</v>
       </c>
@@ -3222,7 +3264,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" ht="14.5" customHeight="1">
       <c r="A95" s="5" t="s">
         <v>39</v>
       </c>
@@ -3242,7 +3284,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" ht="14.5" customHeight="1">
       <c r="A96" s="5" t="s">
         <v>39</v>
       </c>
@@ -3262,7 +3304,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" ht="14.5" customHeight="1">
       <c r="A97" s="5" t="s">
         <v>39</v>
       </c>
@@ -3276,9 +3318,11 @@
         <v>8</v>
       </c>
       <c r="E97" s="11"/>
-      <c r="F97" s="3"/>
-    </row>
-    <row r="98" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F97" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="14.5" customHeight="1">
       <c r="A98" s="5" t="s">
         <v>39</v>
       </c>
@@ -3292,9 +3336,11 @@
         <v>10</v>
       </c>
       <c r="E98" s="11"/>
-      <c r="F98" s="3"/>
-    </row>
-    <row r="99" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F98" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="14.5" customHeight="1">
       <c r="A99" s="5" t="s">
         <v>39</v>
       </c>
@@ -3314,7 +3360,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" ht="14.5" customHeight="1">
       <c r="A100" s="5" t="s">
         <v>39</v>
       </c>
@@ -3334,7 +3380,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" ht="14.5" customHeight="1">
       <c r="A101" s="5" t="s">
         <v>39</v>
       </c>
@@ -3354,7 +3400,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" ht="14.5" customHeight="1">
       <c r="A102" s="5" t="s">
         <v>39</v>
       </c>
@@ -3374,7 +3420,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" ht="14.5" customHeight="1">
       <c r="A103" s="5" t="s">
         <v>39</v>
       </c>
@@ -3394,7 +3440,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" ht="14.5" customHeight="1">
       <c r="A104" s="5" t="s">
         <v>39</v>
       </c>
@@ -3414,7 +3460,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" ht="14.5" customHeight="1">
       <c r="A105" s="5" t="s">
         <v>39</v>
       </c>
@@ -3434,7 +3480,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" ht="14.5" customHeight="1">
       <c r="A106" s="5" t="s">
         <v>39</v>
       </c>
@@ -3454,7 +3500,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6">
       <c r="A107" s="5" t="s">
         <v>39</v>
       </c>
@@ -3474,7 +3520,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6">
       <c r="A108" s="5" t="s">
         <v>39</v>
       </c>
@@ -3494,7 +3540,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6">
       <c r="A109" s="5" t="s">
         <v>39</v>
       </c>
@@ -3514,7 +3560,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6">
       <c r="A110" s="5" t="s">
         <v>39</v>
       </c>
@@ -3534,7 +3580,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6">
       <c r="A111" s="5" t="s">
         <v>39</v>
       </c>
@@ -3554,7 +3600,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6">
       <c r="A112" s="5" t="s">
         <v>39</v>
       </c>
@@ -3574,7 +3620,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6">
       <c r="A113" s="5" t="s">
         <v>39</v>
       </c>
@@ -3594,7 +3640,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6">
       <c r="A114" s="5" t="s">
         <v>39</v>
       </c>
@@ -3614,7 +3660,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6">
       <c r="A115" s="5" t="s">
         <v>39</v>
       </c>
@@ -3625,8 +3671,11 @@
         <v>132</v>
       </c>
       <c r="E115" s="10"/>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F115" s="7" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
       <c r="A116" s="5" t="s">
         <v>39</v>
       </c>
@@ -3637,8 +3686,11 @@
         <v>132</v>
       </c>
       <c r="E116" s="10"/>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F116" s="7" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
       <c r="A117" s="5" t="s">
         <v>39</v>
       </c>
@@ -3649,8 +3701,11 @@
         <v>132</v>
       </c>
       <c r="E117" s="10"/>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F117" s="7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
       <c r="A118" s="5" t="s">
         <v>39</v>
       </c>
@@ -3661,8 +3716,11 @@
         <v>132</v>
       </c>
       <c r="E118" s="10"/>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F118" s="7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
       <c r="A119" s="5" t="s">
         <v>55</v>
       </c>
@@ -3682,7 +3740,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6">
       <c r="A120" s="5" t="s">
         <v>55</v>
       </c>
@@ -3702,7 +3760,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6">
       <c r="A121" s="5" t="s">
         <v>55</v>
       </c>
@@ -3722,7 +3780,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6">
       <c r="A122" s="5" t="s">
         <v>55</v>
       </c>
@@ -3742,7 +3800,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6">
       <c r="A123" s="5" t="s">
         <v>55</v>
       </c>
@@ -3762,7 +3820,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6">
       <c r="A124" s="5" t="s">
         <v>55</v>
       </c>
@@ -3782,7 +3840,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6">
       <c r="A125" s="5" t="s">
         <v>55</v>
       </c>
@@ -3802,7 +3860,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6">
       <c r="A126" s="5" t="s">
         <v>55</v>
       </c>
@@ -3822,7 +3880,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6">
       <c r="A127" s="5" t="s">
         <v>55</v>
       </c>
@@ -3842,7 +3900,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6">
       <c r="A128" s="5" t="s">
         <v>59</v>
       </c>
@@ -3862,7 +3920,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6">
       <c r="A129" s="5" t="s">
         <v>59</v>
       </c>
@@ -3882,7 +3940,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6">
       <c r="A130" s="5" t="s">
         <v>59</v>
       </c>
@@ -3902,7 +3960,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6">
       <c r="A131" s="5" t="s">
         <v>59</v>
       </c>
@@ -3922,7 +3980,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6">
       <c r="A132" s="5" t="s">
         <v>59</v>
       </c>
@@ -3942,7 +4000,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" ht="14.5" customHeight="1">
       <c r="A133" s="5" t="s">
         <v>62</v>
       </c>
@@ -3962,7 +4020,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" ht="14.5" customHeight="1">
       <c r="A134" s="5" t="s">
         <v>62</v>
       </c>
@@ -3982,7 +4040,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" ht="14.5" customHeight="1">
       <c r="A135" s="5" t="s">
         <v>62</v>
       </c>
@@ -4000,7 +4058,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" ht="14.5" customHeight="1">
       <c r="A136" s="5" t="s">
         <v>62</v>
       </c>
@@ -4018,7 +4076,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" ht="14.5" customHeight="1">
       <c r="A137" s="5" t="s">
         <v>62</v>
       </c>
@@ -4036,7 +4094,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" ht="14.5" customHeight="1">
       <c r="A138" s="5" t="s">
         <v>62</v>
       </c>
@@ -4056,7 +4114,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" ht="14.5" customHeight="1">
       <c r="A139" s="5" t="s">
         <v>62</v>
       </c>
@@ -4076,7 +4134,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" ht="14.5" customHeight="1">
       <c r="A140" s="5" t="s">
         <v>62</v>
       </c>
@@ -4096,7 +4154,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" ht="14.5" customHeight="1">
       <c r="A141" s="5" t="s">
         <v>62</v>
       </c>
@@ -4116,7 +4174,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" ht="14.5" customHeight="1">
       <c r="A142" s="5" t="s">
         <v>62</v>
       </c>
@@ -4136,7 +4194,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" ht="14.5" customHeight="1">
       <c r="A143" s="5" t="s">
         <v>62</v>
       </c>
@@ -4156,7 +4214,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6">
       <c r="A144" s="5" t="s">
         <v>62</v>
       </c>
@@ -4176,7 +4234,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6">
       <c r="A145" s="5" t="s">
         <v>62</v>
       </c>
@@ -4196,7 +4254,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6">
       <c r="A146" s="5" t="s">
         <v>62</v>
       </c>
@@ -4216,7 +4274,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6">
       <c r="A147" s="5" t="s">
         <v>62</v>
       </c>
@@ -4236,7 +4294,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6">
       <c r="A148" s="5" t="s">
         <v>62</v>
       </c>
@@ -4256,7 +4314,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6">
       <c r="A149" s="5" t="s">
         <v>62</v>
       </c>
@@ -4276,7 +4334,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6">
       <c r="A150" s="5" t="s">
         <v>62</v>
       </c>
@@ -4296,7 +4354,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6">
       <c r="A151" s="5" t="s">
         <v>62</v>
       </c>
@@ -4316,7 +4374,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6">
       <c r="A152" s="5" t="s">
         <v>62</v>
       </c>
@@ -4336,7 +4394,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6">
       <c r="A153" s="5" t="s">
         <v>62</v>
       </c>
@@ -4356,7 +4414,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6">
       <c r="A154" s="5" t="s">
         <v>62</v>
       </c>
@@ -4376,7 +4434,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6">
       <c r="A155" s="5" t="s">
         <v>62</v>
       </c>
@@ -4396,7 +4454,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6">
       <c r="A156" s="5" t="s">
         <v>62</v>
       </c>
@@ -4416,7 +4474,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6">
       <c r="A157" s="5" t="s">
         <v>62</v>
       </c>
@@ -4436,7 +4494,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6">
       <c r="A158" s="5" t="s">
         <v>62</v>
       </c>
@@ -4456,7 +4514,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6">
       <c r="A159" s="5" t="s">
         <v>62</v>
       </c>
@@ -4476,7 +4534,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="160" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6" s="6" customFormat="1">
       <c r="A160" s="5" t="s">
         <v>72</v>
       </c>
@@ -4496,7 +4554,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="161" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" s="6" customFormat="1">
       <c r="A161" s="5" t="s">
         <v>72</v>
       </c>
@@ -4516,7 +4574,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="162" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" s="6" customFormat="1">
       <c r="A162" s="5" t="s">
         <v>72</v>
       </c>
@@ -4536,7 +4594,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="163" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" s="6" customFormat="1">
       <c r="A163" s="5" t="s">
         <v>72</v>
       </c>
@@ -4556,7 +4614,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="164" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" s="6" customFormat="1">
       <c r="A164" s="5" t="s">
         <v>72</v>
       </c>
@@ -4576,7 +4634,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="165" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" s="6" customFormat="1">
       <c r="A165" s="5" t="s">
         <v>72</v>
       </c>
@@ -4596,7 +4654,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="166" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" s="6" customFormat="1">
       <c r="A166" s="5" t="s">
         <v>72</v>
       </c>
@@ -4616,7 +4674,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="167" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" s="6" customFormat="1">
       <c r="A167" s="5" t="s">
         <v>72</v>
       </c>
@@ -4636,7 +4694,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="168" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" s="6" customFormat="1">
       <c r="A168" s="5" t="s">
         <v>72</v>
       </c>
@@ -4656,7 +4714,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="169" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" s="6" customFormat="1">
       <c r="A169" s="5" t="s">
         <v>72</v>
       </c>
@@ -4676,7 +4734,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="170" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" s="6" customFormat="1">
       <c r="A170" s="5" t="s">
         <v>72</v>
       </c>
@@ -4696,7 +4754,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="171" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" s="6" customFormat="1">
       <c r="A171" s="5" t="s">
         <v>72</v>
       </c>
@@ -4716,7 +4774,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="172" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" s="6" customFormat="1">
       <c r="A172" s="5" t="s">
         <v>72</v>
       </c>
@@ -4736,7 +4794,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="173" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" s="6" customFormat="1">
       <c r="A173" s="5" t="s">
         <v>72</v>
       </c>
@@ -4756,7 +4814,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="174" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:6" s="6" customFormat="1">
       <c r="A174" s="5" t="s">
         <v>72</v>
       </c>
@@ -4776,7 +4834,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6">
       <c r="A175" s="5" t="s">
         <v>77</v>
       </c>
@@ -4796,7 +4854,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6">
       <c r="A176" s="5" t="s">
         <v>77</v>
       </c>
@@ -4816,7 +4874,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:6">
       <c r="A177" s="5" t="s">
         <v>77</v>
       </c>
@@ -4836,7 +4894,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:6">
       <c r="A178" s="5" t="s">
         <v>77</v>
       </c>
@@ -4856,7 +4914,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:6">
       <c r="A179" s="5" t="s">
         <v>77</v>
       </c>
@@ -4876,7 +4934,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:6">
       <c r="A180" s="5" t="s">
         <v>77</v>
       </c>
@@ -4896,7 +4954,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:6">
       <c r="A181" s="5" t="s">
         <v>77</v>
       </c>
@@ -4910,8 +4968,11 @@
         <v>2</v>
       </c>
       <c r="E181" s="10"/>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F181" s="7" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6">
       <c r="A182" s="5" t="s">
         <v>77</v>
       </c>
@@ -4925,8 +4986,11 @@
         <v>3</v>
       </c>
       <c r="E182" s="10"/>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F182" s="7" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6">
       <c r="A183" s="5" t="s">
         <v>77</v>
       </c>
@@ -4946,7 +5010,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:6">
       <c r="A184" s="5" t="s">
         <v>77</v>
       </c>
@@ -4966,7 +5030,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:6">
       <c r="A185" s="5" t="s">
         <v>77</v>
       </c>
@@ -4986,7 +5050,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:6">
       <c r="A186" s="5" t="s">
         <v>77</v>
       </c>
@@ -5006,7 +5070,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:6">
       <c r="A187" s="5" t="s">
         <v>77</v>
       </c>
@@ -5026,7 +5090,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:6">
       <c r="A188" s="5" t="s">
         <v>77</v>
       </c>
@@ -5046,7 +5110,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:6">
       <c r="A189" s="5" t="s">
         <v>77</v>
       </c>
@@ -5060,8 +5124,11 @@
         <v>2</v>
       </c>
       <c r="E189" s="10"/>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F189" s="7" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6">
       <c r="A190" s="5" t="s">
         <v>77</v>
       </c>
@@ -5075,8 +5142,11 @@
         <v>3</v>
       </c>
       <c r="E190" s="10"/>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F190" s="7" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6">
       <c r="A191" s="5" t="s">
         <v>82</v>
       </c>
@@ -5096,7 +5166,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:6">
       <c r="A192" s="5" t="s">
         <v>82</v>
       </c>
@@ -5116,7 +5186,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6">
       <c r="A193" s="5" t="s">
         <v>82</v>
       </c>
@@ -5136,7 +5206,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:6">
       <c r="A194" s="5" t="s">
         <v>82</v>
       </c>
@@ -5156,7 +5226,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6">
       <c r="A195" s="5" t="s">
         <v>85</v>
       </c>
@@ -5176,7 +5246,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:6">
       <c r="A196" s="5" t="s">
         <v>85</v>
       </c>
@@ -5196,7 +5266,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6">
       <c r="A197" s="5" t="s">
         <v>85</v>
       </c>
@@ -5216,7 +5286,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:6">
       <c r="A198" s="5" t="s">
         <v>85</v>
       </c>
@@ -5236,7 +5306,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:6">
       <c r="A199" s="5" t="s">
         <v>85</v>
       </c>
@@ -5256,7 +5326,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6">
       <c r="A200" s="5" t="s">
         <v>85</v>
       </c>
@@ -5276,7 +5346,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6">
       <c r="A201" s="5" t="s">
         <v>85</v>
       </c>
@@ -5290,8 +5360,11 @@
         <v>2</v>
       </c>
       <c r="E201" s="10"/>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F201" s="7" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6">
       <c r="A202" s="5" t="s">
         <v>85</v>
       </c>
@@ -5305,8 +5378,11 @@
         <v>3</v>
       </c>
       <c r="E202" s="10"/>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F202" s="7" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6">
       <c r="A203" s="5" t="s">
         <v>85</v>
       </c>
@@ -5317,8 +5393,11 @@
         <v>132</v>
       </c>
       <c r="E203" s="10"/>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F203" s="7" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6">
       <c r="A204" s="5" t="s">
         <v>88</v>
       </c>
@@ -5338,7 +5417,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:6">
       <c r="A205" s="5" t="s">
         <v>88</v>
       </c>
@@ -5358,7 +5437,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:6">
       <c r="A206" s="5" t="s">
         <v>88</v>
       </c>
@@ -5378,7 +5457,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:6">
       <c r="A207" s="5" t="s">
         <v>88</v>
       </c>
@@ -5398,7 +5477,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:6">
       <c r="A208" s="5" t="s">
         <v>88</v>
       </c>
@@ -5418,7 +5497,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:6">
       <c r="A209" s="5" t="s">
         <v>88</v>
       </c>
@@ -5438,7 +5517,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:6">
       <c r="A210" s="5" t="s">
         <v>88</v>
       </c>
@@ -5458,7 +5537,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:6">
       <c r="A211" s="5" t="s">
         <v>88</v>
       </c>
@@ -5478,7 +5557,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:6">
       <c r="A212" s="5" t="s">
         <v>93</v>
       </c>
@@ -5498,7 +5577,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:6">
       <c r="A213" s="5" t="s">
         <v>93</v>
       </c>
@@ -5518,7 +5597,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:6">
       <c r="A214" s="5" t="s">
         <v>93</v>
       </c>
@@ -5538,7 +5617,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:6">
       <c r="A215" s="5" t="s">
         <v>93</v>
       </c>
@@ -5558,7 +5637,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:6">
       <c r="A216" s="5" t="s">
         <v>93</v>
       </c>
@@ -5578,7 +5657,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:6">
       <c r="A217" s="5" t="s">
         <v>93</v>
       </c>
@@ -5598,7 +5677,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:6">
       <c r="A218" s="5" t="s">
         <v>93</v>
       </c>
@@ -5618,7 +5697,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:6">
       <c r="A219" s="5" t="s">
         <v>93</v>
       </c>
@@ -5638,7 +5717,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:6">
       <c r="A220" s="5" t="s">
         <v>93</v>
       </c>
@@ -5658,7 +5737,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:6">
       <c r="A221" s="5" t="s">
         <v>93</v>
       </c>
@@ -5678,7 +5757,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:6">
       <c r="A222" s="5" t="s">
         <v>93</v>
       </c>
@@ -5698,7 +5777,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:6">
       <c r="A223" s="5" t="s">
         <v>93</v>
       </c>
@@ -5718,7 +5797,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:6">
       <c r="A224" s="5" t="s">
         <v>93</v>
       </c>
@@ -5738,7 +5817,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:6">
       <c r="A225" s="5" t="s">
         <v>93</v>
       </c>
@@ -5758,7 +5837,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:6">
       <c r="A226" s="5" t="s">
         <v>93</v>
       </c>
@@ -5778,7 +5857,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:6">
       <c r="A227" s="5" t="s">
         <v>93</v>
       </c>
@@ -5798,7 +5877,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:6">
       <c r="A228" s="5" t="s">
         <v>93</v>
       </c>
@@ -5818,7 +5897,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:6">
       <c r="A229" s="5" t="s">
         <v>93</v>
       </c>
@@ -5838,7 +5917,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:6">
       <c r="A230" s="5" t="s">
         <v>93</v>
       </c>
@@ -5858,7 +5937,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:6">
       <c r="A231" s="5" t="s">
         <v>93</v>
       </c>
@@ -5878,7 +5957,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:6">
       <c r="A232" s="5" t="s">
         <v>93</v>
       </c>
@@ -5898,7 +5977,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:6">
       <c r="A233" s="5" t="s">
         <v>93</v>
       </c>
@@ -5918,7 +5997,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="234" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:6" s="6" customFormat="1">
       <c r="A234" s="5" t="s">
         <v>101</v>
       </c>
@@ -5938,7 +6017,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="235" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:6" s="6" customFormat="1">
       <c r="A235" s="5" t="s">
         <v>101</v>
       </c>
@@ -5958,7 +6037,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="236" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:6" s="6" customFormat="1">
       <c r="A236" s="5" t="s">
         <v>101</v>
       </c>
@@ -5978,7 +6057,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="237" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:6" s="6" customFormat="1">
       <c r="A237" s="5" t="s">
         <v>101</v>
       </c>
@@ -5998,7 +6077,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="238" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:6" s="6" customFormat="1">
       <c r="A238" s="5" t="s">
         <v>101</v>
       </c>
@@ -6018,7 +6097,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="239" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:6" s="6" customFormat="1">
       <c r="A239" s="5" t="s">
         <v>101</v>
       </c>
@@ -6038,7 +6117,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="240" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:6" s="6" customFormat="1">
       <c r="A240" s="5" t="s">
         <v>101</v>
       </c>
@@ -6058,7 +6137,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="241" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:6" s="6" customFormat="1">
       <c r="A241" s="5" t="s">
         <v>101</v>
       </c>
@@ -6078,7 +6157,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="242" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:6" s="6" customFormat="1">
       <c r="A242" s="5" t="s">
         <v>101</v>
       </c>
@@ -6098,7 +6177,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="243" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:6" s="6" customFormat="1">
       <c r="A243" s="5" t="s">
         <v>101</v>
       </c>
@@ -6118,7 +6197,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:6">
       <c r="A244" s="5" t="s">
         <v>106</v>
       </c>
@@ -6138,7 +6217,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:6">
       <c r="A245" s="5" t="s">
         <v>106</v>
       </c>
@@ -6158,7 +6237,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:6">
       <c r="A246" s="5" t="s">
         <v>106</v>
       </c>
@@ -6178,7 +6257,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:6">
       <c r="A247" s="5" t="s">
         <v>106</v>
       </c>
@@ -6198,7 +6277,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:6">
       <c r="A248" s="5" t="s">
         <v>106</v>
       </c>
@@ -6218,7 +6297,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:6">
       <c r="A249" s="5" t="s">
         <v>106</v>
       </c>
@@ -6238,7 +6317,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:6">
       <c r="A250" s="5" t="s">
         <v>106</v>
       </c>
@@ -6258,7 +6337,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:6">
       <c r="A251" s="5" t="s">
         <v>106</v>
       </c>
@@ -6278,7 +6357,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:6">
       <c r="A252" s="5" t="s">
         <v>106</v>
       </c>
@@ -6298,7 +6377,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:6">
       <c r="A253" s="5" t="s">
         <v>106</v>
       </c>
@@ -6318,7 +6397,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:6">
       <c r="A254" s="5" t="s">
         <v>106</v>
       </c>
@@ -6338,7 +6417,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:6">
       <c r="A255" s="5" t="s">
         <v>106</v>
       </c>
@@ -6358,7 +6437,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:6">
       <c r="A256" s="5" t="s">
         <v>106</v>
       </c>
@@ -6378,7 +6457,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="257" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:6" ht="14.5" customHeight="1">
       <c r="A257" s="5" t="s">
         <v>111</v>
       </c>
@@ -6398,7 +6477,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="258" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:6" ht="14.5" customHeight="1">
       <c r="A258" s="5" t="s">
         <v>111</v>
       </c>
@@ -6418,7 +6497,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="259" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:6" ht="14.5" customHeight="1">
       <c r="A259" s="5" t="s">
         <v>111</v>
       </c>
@@ -6438,7 +6517,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="260" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:6" ht="14.5" customHeight="1">
       <c r="A260" s="5" t="s">
         <v>111</v>
       </c>
@@ -6458,7 +6537,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="261" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:6" ht="14.5" customHeight="1">
       <c r="A261" s="5" t="s">
         <v>111</v>
       </c>
@@ -6478,7 +6557,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="262" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:6" ht="14.5" customHeight="1">
       <c r="A262" s="5" t="s">
         <v>111</v>
       </c>
@@ -6498,7 +6577,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="263" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:6" ht="14.5" customHeight="1">
       <c r="A263" s="5" t="s">
         <v>111</v>
       </c>
@@ -6518,7 +6597,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="264" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:6" ht="14.5" customHeight="1">
       <c r="A264" s="5" t="s">
         <v>111</v>
       </c>
@@ -6538,7 +6617,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="265" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:6" ht="14.5" customHeight="1">
       <c r="A265" s="5" t="s">
         <v>111</v>
       </c>
@@ -6558,7 +6637,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="266" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:6" ht="14.5" customHeight="1">
       <c r="A266" s="5" t="s">
         <v>111</v>
       </c>
@@ -6578,7 +6657,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="267" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:6" ht="14.5" customHeight="1">
       <c r="A267" s="5" t="s">
         <v>111</v>
       </c>
@@ -6598,7 +6677,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="268" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:6" ht="14.5" customHeight="1">
       <c r="A268" s="5" t="s">
         <v>111</v>
       </c>
@@ -6618,7 +6697,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="269" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:6" s="3" customFormat="1">
       <c r="A269" s="3" t="s">
         <v>261</v>
       </c>
@@ -6634,8 +6713,11 @@
       <c r="E269" s="8" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="270" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F269" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" s="3" customFormat="1">
       <c r="A270" s="3" t="s">
         <v>261</v>
       </c>
@@ -6651,8 +6733,11 @@
       <c r="E270" s="8" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="271" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F270" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" s="3" customFormat="1">
       <c r="A271" s="3" t="s">
         <v>265</v>
       </c>
@@ -6670,7 +6755,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="272" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:6" s="3" customFormat="1">
       <c r="A272" s="3" t="s">
         <v>265</v>
       </c>
@@ -6688,7 +6773,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="273" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:6" s="3" customFormat="1">
       <c r="A273" s="3" t="s">
         <v>285</v>
       </c>
@@ -6708,7 +6793,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="274" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:6" s="3" customFormat="1">
       <c r="A274" s="3" t="s">
         <v>285</v>
       </c>
@@ -6728,7 +6813,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="275" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:6" s="3" customFormat="1">
       <c r="A275" s="3" t="s">
         <v>285</v>
       </c>
@@ -6748,7 +6833,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="276" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:6" s="3" customFormat="1">
       <c r="A276" s="3" t="s">
         <v>285</v>
       </c>

</xml_diff>